<commit_message>
faz algumas correções de data nos gráficos e correçÕes no vba
</commit_message>
<xml_diff>
--- a/doc/SUZB3sg_1ano.xlsx
+++ b/doc/SUZB3sg_1ano.xlsx
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C242"/>
+  <dimension ref="A1:C248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -406,2652 +406,2718 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2">
-        <v>45414</v>
+        <v>45422</v>
       </c>
       <c r="B2">
-        <v>-0.002704073009971331</v>
+        <v>0.01972386587771213</v>
       </c>
       <c r="C2">
-        <v>0.009513674915028192</v>
+        <v>-0.004587012824913361</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2">
-        <v>45412</v>
+        <v>45421</v>
       </c>
       <c r="B3">
-        <v>-0.009320454160311797</v>
+        <v>0.01934235976789167</v>
       </c>
       <c r="C3">
-        <v>-0.01121301589295809</v>
+        <v>-0.009986021115067079</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2">
-        <v>45411</v>
+        <v>45420</v>
       </c>
       <c r="B4">
-        <v>0.007526513855627748</v>
+        <v>-0.007210626185958358</v>
       </c>
       <c r="C4">
-        <v>0.006528302483284065</v>
+        <v>0.002097360885380484</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2">
-        <v>45408</v>
+        <v>45419</v>
       </c>
       <c r="B5">
-        <v>0.01154499151103572</v>
+        <v>-0.002675840978593302</v>
       </c>
       <c r="C5">
-        <v>0.0150827142467469</v>
+        <v>0.0057914156274812</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2">
-        <v>45407</v>
+        <v>45418</v>
       </c>
       <c r="B6">
-        <v>0.005370929842228866</v>
+        <v>0.1399003449597547</v>
       </c>
       <c r="C6">
-        <v>-0.0007615779895944197</v>
+        <v>-0.0003346069146907826</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2">
-        <v>45406</v>
+        <v>45415</v>
       </c>
       <c r="B7">
-        <v>0.01101836393989997</v>
+        <v>-0.005211835911230533</v>
       </c>
       <c r="C7">
-        <v>-0.003252149455045261</v>
+        <v>0.01091077862211098</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2">
-        <v>45405</v>
+        <v>45414</v>
       </c>
       <c r="B8">
-        <v>-0.007265521796565477</v>
+        <v>-0.002704073009971331</v>
       </c>
       <c r="C8">
-        <v>-0.003384485518383773</v>
+        <v>0.009513674915028192</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2">
-        <v>45404</v>
+        <v>45412</v>
       </c>
       <c r="B9">
-        <v>0.007152361942781127</v>
+        <v>-0.009320454160311797</v>
       </c>
       <c r="C9">
-        <v>0.0035884402672548</v>
+        <v>-0.01121301589295809</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2">
-        <v>45401</v>
+        <v>45411</v>
       </c>
       <c r="B10">
-        <v>0.0109000825763832</v>
+        <v>0.007526513855627748</v>
       </c>
       <c r="C10">
-        <v>0.007472060291796812</v>
+        <v>0.006528302483284065</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2">
-        <v>45400</v>
+        <v>45408</v>
       </c>
       <c r="B11">
-        <v>-0.007515111909818684</v>
+        <v>0.01154499151103572</v>
       </c>
       <c r="C11">
-        <v>0.0002013352554139924</v>
+        <v>0.0150827142467469</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2">
-        <v>45399</v>
+        <v>45407</v>
       </c>
       <c r="B12">
-        <v>0.0009876543209876854</v>
+        <v>0.005370929842228866</v>
       </c>
       <c r="C12">
-        <v>-0.001752566545273337</v>
+        <v>-0.0007615779895944197</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2">
-        <v>45398</v>
+        <v>45406</v>
       </c>
       <c r="B13">
-        <v>0.008880118401578763</v>
+        <v>0.01101836393989997</v>
       </c>
       <c r="C13">
-        <v>-0.007539853511417505</v>
+        <v>-0.003252149455045261</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2">
-        <v>45397</v>
+        <v>45405</v>
       </c>
       <c r="B14">
-        <v>-0.004889975550122272</v>
+        <v>-0.007265521796565477</v>
       </c>
       <c r="C14">
-        <v>-0.004859225382306653</v>
+        <v>-0.003384485518383773</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2">
-        <v>45394</v>
+        <v>45404</v>
       </c>
       <c r="B15">
-        <v>0.002457002457002533</v>
+        <v>0.007152361942781127</v>
       </c>
       <c r="C15">
-        <v>-0.01138183302458473</v>
+        <v>0.0035884402672548</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2">
-        <v>45393</v>
+        <v>45401</v>
       </c>
       <c r="B16">
-        <v>0.0001633986928104569</v>
+        <v>0.0109000825763832</v>
       </c>
       <c r="C16">
-        <v>-0.005138457213363146</v>
+        <v>0.007472060291796812</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="2">
-        <v>45392</v>
+        <v>45400</v>
       </c>
       <c r="B17">
-        <v>0.008985459892174363</v>
+        <v>-0.007515111909818684</v>
       </c>
       <c r="C17">
-        <v>-0.01413503733928712</v>
+        <v>0.0002013352554139924</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2">
-        <v>45391</v>
+        <v>45399</v>
       </c>
       <c r="B18">
-        <v>0.0085816062176165</v>
+        <v>0.0009876543209876854</v>
       </c>
       <c r="C18">
-        <v>0.008016638599377623</v>
+        <v>-0.001752566545273337</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2">
-        <v>45390</v>
+        <v>45398</v>
       </c>
       <c r="B19">
-        <v>0.004976721785198368</v>
+        <v>0.008880118401578763</v>
       </c>
       <c r="C19">
-        <v>0.0162624709176229</v>
+        <v>-0.007539853511417505</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2">
-        <v>45387</v>
+        <v>45397</v>
       </c>
       <c r="B20">
-        <v>0.003354632587859507</v>
+        <v>-0.004889975550122272</v>
       </c>
       <c r="C20">
-        <v>-0.004967511065072094</v>
+        <v>-0.004859225382306653</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2">
-        <v>45386</v>
+        <v>45394</v>
       </c>
       <c r="B21">
-        <v>0.01703550390065267</v>
+        <v>0.002457002457002533</v>
       </c>
       <c r="C21">
-        <v>0.000863978384831654</v>
+        <v>-0.01138183302458473</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2">
-        <v>45385</v>
+        <v>45393</v>
       </c>
       <c r="B22">
-        <v>0.01127113337507812</v>
+        <v>0.0001633986928104569</v>
       </c>
       <c r="C22">
-        <v>-0.001811068687328055</v>
+        <v>-0.005138457213363146</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2">
-        <v>45384</v>
+        <v>45392</v>
       </c>
       <c r="B23">
-        <v>0.009752321981424394</v>
+        <v>0.008985459892174363</v>
       </c>
       <c r="C23">
-        <v>0.004401921411134824</v>
+        <v>-0.01413503733928712</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="2">
-        <v>45383</v>
+        <v>45391</v>
       </c>
       <c r="B24">
-        <v>-0.005212325617047431</v>
+        <v>0.0085816062176165</v>
       </c>
       <c r="C24">
-        <v>-0.008711535759449163</v>
+        <v>0.008016638599377623</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2">
-        <v>45379</v>
+        <v>45390</v>
       </c>
       <c r="B25">
-        <v>-0.0140237324703345</v>
+        <v>0.004976721785198368</v>
       </c>
       <c r="C25">
-        <v>0.003250033283473286</v>
+        <v>0.0162624709176229</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2">
-        <v>45378</v>
+        <v>45387</v>
       </c>
       <c r="B26">
-        <v>-0.002813379180994002</v>
+        <v>0.003354632587859507</v>
       </c>
       <c r="C26">
-        <v>0.006526725680458423</v>
+        <v>-0.004967511065072094</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2">
-        <v>45377</v>
+        <v>45386</v>
       </c>
       <c r="B27">
-        <v>-0.01300940438871467</v>
+        <v>0.01703550390065267</v>
       </c>
       <c r="C27">
-        <v>-0.000535724133584381</v>
+        <v>0.000863978384831654</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="2">
-        <v>45376</v>
+        <v>45385</v>
       </c>
       <c r="B28">
-        <v>-0.02143878037160551</v>
+        <v>0.01127113337507812</v>
       </c>
       <c r="C28">
-        <v>-0.0007557448416478652</v>
+        <v>-0.001811068687328055</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="2">
-        <v>45373</v>
+        <v>45384</v>
       </c>
       <c r="B29">
-        <v>0.0004829362524148006</v>
+        <v>0.009752321981424394</v>
       </c>
       <c r="C29">
-        <v>-0.008832778033536437</v>
+        <v>0.004401921411134824</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="2">
-        <v>45372</v>
+        <v>45383</v>
       </c>
       <c r="B30">
-        <v>-0.001769911504424737</v>
+        <v>-0.005212325617047431</v>
       </c>
       <c r="C30">
-        <v>-0.007481122942884832</v>
+        <v>-0.008711535759449163</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="2">
-        <v>45371</v>
+        <v>45379</v>
       </c>
       <c r="B31">
-        <v>0.0003223726627983314</v>
+        <v>-0.0140237324703345</v>
       </c>
       <c r="C31">
-        <v>0.01251480055516785</v>
+        <v>0.003250033283473286</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2">
-        <v>45370</v>
+        <v>45378</v>
       </c>
       <c r="B32">
-        <v>0.01272961650016113</v>
+        <v>-0.002813379180994002</v>
       </c>
       <c r="C32">
-        <v>0.004529199552593788</v>
+        <v>0.006526725680458423</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="2">
-        <v>45369</v>
+        <v>45377</v>
       </c>
       <c r="B33">
-        <v>-0.02863961813842486</v>
+        <v>-0.01300940438871467</v>
       </c>
       <c r="C33">
-        <v>0.001672689400514349</v>
+        <v>-0.000535724133584381</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="2">
-        <v>45366</v>
+        <v>45376</v>
       </c>
       <c r="B34">
-        <v>-0.004095004095004073</v>
+        <v>-0.02143878037160551</v>
       </c>
       <c r="C34">
-        <v>-0.007424230558383593</v>
+        <v>-0.0007557448416478652</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="2">
-        <v>45365</v>
+        <v>45373</v>
       </c>
       <c r="B35">
-        <v>-0.02138157894736836</v>
+        <v>0.0004829362524148006</v>
       </c>
       <c r="C35">
-        <v>-0.002468634282768001</v>
+        <v>-0.008832778033536437</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2">
-        <v>45364</v>
+        <v>45372</v>
       </c>
       <c r="B36">
-        <v>-0.001176470588235334</v>
+        <v>-0.001769911504424737</v>
       </c>
       <c r="C36">
-        <v>0.002647491932199042</v>
+        <v>-0.007481122942884832</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="2">
-        <v>45363</v>
+        <v>45371</v>
       </c>
       <c r="B37">
-        <v>-0.005384485949856965</v>
+        <v>0.0003223726627983314</v>
       </c>
       <c r="C37">
-        <v>0.01224192064951946</v>
+        <v>0.01251480055516785</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="2">
-        <v>45362</v>
+        <v>45370</v>
       </c>
       <c r="B38">
-        <v>-0.00913551006597868</v>
+        <v>0.01272961650016113</v>
       </c>
       <c r="C38">
-        <v>-0.007452526540280613</v>
+        <v>0.004529199552593788</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="2">
-        <v>45359</v>
+        <v>45369</v>
       </c>
       <c r="B39">
-        <v>0.009902680553184107</v>
+        <v>-0.02863961813842486</v>
       </c>
       <c r="C39">
-        <v>-0.009887798036465667</v>
+        <v>0.001672689400514349</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="2">
-        <v>45358</v>
+        <v>45366</v>
       </c>
       <c r="B40">
-        <v>-0.005579036348267064</v>
+        <v>-0.004095004095004073</v>
       </c>
       <c r="C40">
-        <v>-0.004267204593063845</v>
+        <v>-0.007424230558383593</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="2">
-        <v>45357</v>
+        <v>45365</v>
       </c>
       <c r="B41">
-        <v>-0.009010540632438002</v>
+        <v>-0.02138157894736836</v>
       </c>
       <c r="C41">
-        <v>0.006182766319536626</v>
+        <v>-0.002468634282768001</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="2">
-        <v>45356</v>
+        <v>45364</v>
       </c>
       <c r="B42">
-        <v>0.00480356836507112</v>
+        <v>-0.001176470588235334</v>
       </c>
       <c r="C42">
-        <v>-0.001893393381694031</v>
+        <v>0.002647491932199042</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="2">
-        <v>45355</v>
+        <v>45363</v>
       </c>
       <c r="B43">
-        <v>-0.002048830459279505</v>
+        <v>-0.005384485949856965</v>
       </c>
       <c r="C43">
-        <v>-0.006494813438612801</v>
+        <v>0.01224192064951946</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="2">
-        <v>45352</v>
+        <v>45362</v>
       </c>
       <c r="B44">
-        <v>-0.0164242942686057</v>
+        <v>-0.00913551006597868</v>
       </c>
       <c r="C44">
-        <v>0.001240117811192043</v>
+        <v>-0.007452526540280613</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="2">
-        <v>45351</v>
+        <v>45359</v>
       </c>
       <c r="B45">
-        <v>-0.01982953557140377</v>
+        <v>0.009902680553184107</v>
       </c>
       <c r="C45">
-        <v>-0.008720371864315624</v>
+        <v>-0.009887798036465667</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="2">
-        <v>45350</v>
+        <v>45358</v>
       </c>
       <c r="B46">
-        <v>0.01827861579414369</v>
+        <v>-0.005579036348267064</v>
       </c>
       <c r="C46">
-        <v>-0.01164865706323226</v>
+        <v>-0.004267204593063845</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="2">
-        <v>45349</v>
+        <v>45357</v>
       </c>
       <c r="B47">
-        <v>-0.009759498082955731</v>
+        <v>-0.009010540632438002</v>
       </c>
       <c r="C47">
-        <v>0.01604826825297634</v>
+        <v>0.006182766319536626</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="2">
-        <v>45348</v>
+        <v>45356</v>
       </c>
       <c r="B48">
-        <v>-0.01231960577261537</v>
+        <v>0.00480356836507112</v>
       </c>
       <c r="C48">
-        <v>0.001468099738060058</v>
+        <v>-0.001893393381694031</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="2">
-        <v>45345</v>
+        <v>45355</v>
       </c>
       <c r="B49">
-        <v>-0.01514611546685662</v>
+        <v>-0.002048830459279505</v>
       </c>
       <c r="C49">
-        <v>-0.006311376601838115</v>
+        <v>-0.006494813438612801</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="2">
-        <v>45344</v>
+        <v>45352</v>
       </c>
       <c r="B50">
-        <v>0.00850370906459208</v>
+        <v>-0.0164242942686057</v>
       </c>
       <c r="C50">
-        <v>0.001607296665436131</v>
+        <v>0.001240117811192043</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="2">
-        <v>45343</v>
+        <v>45351</v>
       </c>
       <c r="B51">
-        <v>-0.008432005740940052</v>
+        <v>-0.01982953557140377</v>
       </c>
       <c r="C51">
-        <v>0.0008928846331475171</v>
+        <v>-0.008720371864315624</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="2">
-        <v>45342</v>
+        <v>45350</v>
       </c>
       <c r="B52">
-        <v>-0.02533019721367846</v>
+        <v>0.01827861579414369</v>
       </c>
       <c r="C52">
-        <v>0.006819802225735527</v>
+        <v>-0.01164865706323226</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="2">
-        <v>45341</v>
+        <v>45349</v>
       </c>
       <c r="B53">
-        <v>-0.0154074624095043</v>
+        <v>-0.009759498082955731</v>
       </c>
       <c r="C53">
-        <v>0.002408215900439714</v>
+        <v>0.01604826825297634</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="2">
-        <v>45338</v>
+        <v>45348</v>
       </c>
       <c r="B54">
-        <v>0.0001885369532428349</v>
+        <v>-0.01231960577261537</v>
       </c>
       <c r="C54">
-        <v>0.007214171700416161</v>
+        <v>0.001468099738060058</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="2">
-        <v>45337</v>
+        <v>45345</v>
       </c>
       <c r="B55">
-        <v>-0.0133836003770027</v>
+        <v>-0.01514611546685662</v>
       </c>
       <c r="C55">
-        <v>0.006188099324505147</v>
+        <v>-0.006311376601838115</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="2">
-        <v>45336</v>
+        <v>45344</v>
       </c>
       <c r="B56">
-        <v>-0.001719526175009589</v>
+        <v>0.00850370906459208</v>
       </c>
       <c r="C56">
-        <v>-0.007873400715479706</v>
+        <v>0.001607296665436131</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="2">
-        <v>45331</v>
+        <v>45343</v>
       </c>
       <c r="B57">
-        <v>0.008612440191387627</v>
+        <v>-0.008432005740940052</v>
       </c>
       <c r="C57">
-        <v>-0.001489662057293506</v>
+        <v>0.0008928846331475171</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="2">
-        <v>45330</v>
+        <v>45342</v>
       </c>
       <c r="B58">
-        <v>0.01423149905123333</v>
+        <v>-0.02533019721367846</v>
       </c>
       <c r="C58">
-        <v>-0.01073236219986418</v>
+        <v>0.006819802225735527</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="2">
-        <v>45329</v>
+        <v>45341</v>
       </c>
       <c r="B59">
-        <v>0.00467726847521055</v>
+        <v>-0.0154074624095043</v>
       </c>
       <c r="C59">
-        <v>-0.006195558827137737</v>
+        <v>0.002408215900439714</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="2">
-        <v>45328</v>
+        <v>45338</v>
       </c>
       <c r="B60">
-        <v>0.000186219739292337</v>
+        <v>0.0001885369532428349</v>
       </c>
       <c r="C60">
-        <v>0.02212503820742517</v>
+        <v>0.007214171700416161</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="2">
-        <v>45327</v>
+        <v>45337</v>
       </c>
       <c r="B61">
-        <v>-0.03649227331967975</v>
+        <v>-0.0133836003770027</v>
       </c>
       <c r="C61">
-        <v>0.003231589375854993</v>
+        <v>0.006188099324505147</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="2">
-        <v>45324</v>
+        <v>45336</v>
       </c>
       <c r="B62">
-        <v>-0.007922705314009626</v>
+        <v>-0.001719526175009589</v>
       </c>
       <c r="C62">
-        <v>-0.01011044434585662</v>
+        <v>-0.007873400715479706</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="2">
-        <v>45323</v>
+        <v>45331</v>
       </c>
       <c r="B63">
-        <v>-0.004674717569146947</v>
+        <v>0.008612440191387627</v>
       </c>
       <c r="C63">
-        <v>0.00570636858914142</v>
+        <v>-0.001489662057293506</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="2">
-        <v>45322</v>
+        <v>45330</v>
       </c>
       <c r="B64">
-        <v>0.01017612524461842</v>
+        <v>0.01423149905123333</v>
       </c>
       <c r="C64">
-        <v>0.002747209619943236</v>
+        <v>-0.01073236219986418</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="2">
-        <v>45321</v>
+        <v>45329</v>
       </c>
       <c r="B65">
-        <v>0.009298721425804013</v>
+        <v>0.00467726847521055</v>
       </c>
       <c r="C65">
-        <v>-0.008567893356575373</v>
+        <v>-0.006195558827137737</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="2">
-        <v>45320</v>
+        <v>45328</v>
       </c>
       <c r="B66">
-        <v>-0.0249520153550864</v>
+        <v>0.000186219739292337</v>
       </c>
       <c r="C66">
-        <v>-0.003597819597261354</v>
+        <v>0.02212503820742517</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="2">
-        <v>45317</v>
+        <v>45327</v>
       </c>
       <c r="B67">
-        <v>0.04153543307086616</v>
+        <v>-0.03649227331967975</v>
       </c>
       <c r="C67">
-        <v>0.006226154530346584</v>
+        <v>0.003231589375854993</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="2">
-        <v>45316</v>
+        <v>45324</v>
       </c>
       <c r="B68">
-        <v>-0.02003402003401999</v>
+        <v>-0.007922705314009626</v>
       </c>
       <c r="C68">
-        <v>0.002761782562433535</v>
+        <v>-0.01011044434585662</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="2">
-        <v>45315</v>
+        <v>45323</v>
       </c>
       <c r="B69">
-        <v>0.0003857280617163283</v>
+        <v>-0.004674717569146947</v>
       </c>
       <c r="C69">
-        <v>-0.003485026858875861</v>
+        <v>0.00570636858914142</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="2">
-        <v>45314</v>
+        <v>45322</v>
       </c>
       <c r="B70">
-        <v>0.00443416232889926</v>
+        <v>0.01017612524461842</v>
       </c>
       <c r="C70">
-        <v>0.01311985592644671</v>
+        <v>0.002747209619943236</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="2">
-        <v>45313</v>
+        <v>45321</v>
       </c>
       <c r="B71">
-        <v>-0.008253358925143894</v>
+        <v>0.009298721425804013</v>
       </c>
       <c r="C71">
-        <v>-0.008101162681375174</v>
+        <v>-0.008567893356575373</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="2">
-        <v>45310</v>
+        <v>45320</v>
       </c>
       <c r="B72">
-        <v>0.002515966711824857</v>
+        <v>-0.0249520153550864</v>
       </c>
       <c r="C72">
-        <v>0.002513431147695533</v>
+        <v>-0.003597819597261354</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="2">
-        <v>45309</v>
+        <v>45317</v>
       </c>
       <c r="B73">
-        <v>-0.005212355212355191</v>
+        <v>0.04153543307086616</v>
       </c>
       <c r="C73">
-        <v>-0.009399022750614661</v>
+        <v>0.006226154530346584</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="2">
-        <v>45308</v>
+        <v>45316</v>
       </c>
       <c r="B74">
-        <v>0.02270522026004262</v>
+        <v>-0.02003402003401999</v>
       </c>
       <c r="C74">
-        <v>-0.005955419431682873</v>
+        <v>0.002761782562433535</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="2">
-        <v>45307</v>
+        <v>45315</v>
       </c>
       <c r="B75">
-        <v>0.004174573055028441</v>
+        <v>0.0003857280617163283</v>
       </c>
       <c r="C75">
-        <v>-0.01693265714220538</v>
+        <v>-0.003485026858875861</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="2">
-        <v>45306</v>
+        <v>45314</v>
       </c>
       <c r="B76">
-        <v>0.01776266061980336</v>
+        <v>0.00443416232889926</v>
       </c>
       <c r="C76">
-        <v>0.004069075029773828</v>
+        <v>0.01311985592644671</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="2">
-        <v>45303</v>
+        <v>45313</v>
       </c>
       <c r="B77">
-        <v>-0.00519866320089124</v>
+        <v>-0.008253358925143894</v>
       </c>
       <c r="C77">
-        <v>0.00259473857434811</v>
+        <v>-0.008101162681375174</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="2">
-        <v>45302</v>
+        <v>45310</v>
       </c>
       <c r="B78">
-        <v>0.01082493467711831</v>
+        <v>0.002515966711824857</v>
       </c>
       <c r="C78">
-        <v>-0.00146742993404203</v>
+        <v>0.002513431147695533</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="2">
-        <v>45301</v>
+        <v>45309</v>
       </c>
       <c r="B79">
-        <v>-0.007200886262924588</v>
+        <v>-0.005212355212355191</v>
       </c>
       <c r="C79">
-        <v>-0.004610223131756519</v>
+        <v>-0.009399022750614661</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="2">
-        <v>45300</v>
+        <v>45308</v>
       </c>
       <c r="B80">
-        <v>0.005765296633810646</v>
+        <v>0.02270522026004262</v>
       </c>
       <c r="C80">
-        <v>-0.007400303563472654</v>
+        <v>-0.005955419431682873</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="2">
-        <v>45299</v>
+        <v>45307</v>
       </c>
       <c r="B81">
-        <v>0.01238905325443795</v>
+        <v>0.004174573055028441</v>
       </c>
       <c r="C81">
-        <v>0.003060072866091446</v>
+        <v>-0.01693265714220538</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="2">
-        <v>45296</v>
+        <v>45306</v>
       </c>
       <c r="B82">
-        <v>-0.0127853881278539</v>
+        <v>0.01776266061980336</v>
       </c>
       <c r="C82">
-        <v>0.006073491533689968</v>
+        <v>0.004069075029773828</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="2">
-        <v>45295</v>
+        <v>45303</v>
       </c>
       <c r="B83">
-        <v>0.01036077705827942</v>
+        <v>-0.00519866320089124</v>
       </c>
       <c r="C83">
-        <v>-0.01210533447761863</v>
+        <v>0.00259473857434811</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="2">
-        <v>45294</v>
+        <v>45302</v>
       </c>
       <c r="B84">
-        <v>0.01538179820545693</v>
+        <v>0.01082493467711831</v>
       </c>
       <c r="C84">
-        <v>0.001032427259094026</v>
+        <v>-0.00146742993404203</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="2">
-        <v>45293</v>
+        <v>45301</v>
       </c>
       <c r="B85">
-        <v>-0.005590622182146121</v>
+        <v>-0.007200886262924588</v>
       </c>
       <c r="C85">
-        <v>-0.01108916793978465</v>
+        <v>-0.004610223131756519</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="2">
-        <v>45288</v>
+        <v>45300</v>
       </c>
       <c r="B86">
-        <v>0.00888647080159588</v>
+        <v>0.005765296633810646</v>
       </c>
       <c r="C86">
-        <v>-6.706708198578326E-05</v>
+        <v>-0.007400303563472654</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="2">
-        <v>45287</v>
+        <v>45299</v>
       </c>
       <c r="B87">
-        <v>-0.001438072982203997</v>
+        <v>0.01238905325443795</v>
       </c>
       <c r="C87">
-        <v>0.004950087244351531</v>
+        <v>0.003060072866091446</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="2">
-        <v>45286</v>
+        <v>45296</v>
       </c>
       <c r="B88">
-        <v>-0.005940594059405946</v>
+        <v>-0.0127853881278539</v>
       </c>
       <c r="C88">
-        <v>0.005875573433368642</v>
+        <v>0.006073491533689968</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="2">
-        <v>45282</v>
+        <v>45295</v>
       </c>
       <c r="B89">
-        <v>-0.005070626584570803</v>
+        <v>0.01036077705827942</v>
       </c>
       <c r="C89">
-        <v>0.00431980148583011</v>
+        <v>-0.01210533447761863</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="2">
-        <v>45281</v>
+        <v>45294</v>
       </c>
       <c r="B90">
-        <v>-0.008918820531488847</v>
+        <v>0.01538179820545693</v>
       </c>
       <c r="C90">
-        <v>0.01053484602917343</v>
+        <v>0.001032427259094026</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="2">
-        <v>45280</v>
+        <v>45293</v>
       </c>
       <c r="B91">
-        <v>-0.01010101010101017</v>
+        <v>-0.005590622182146121</v>
       </c>
       <c r="C91">
-        <v>-0.007940781639881433</v>
+        <v>-0.01108916793978465</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="2">
-        <v>45279</v>
+        <v>45288</v>
       </c>
       <c r="B92">
-        <v>-0.01725417439703159</v>
+        <v>0.00888647080159588</v>
       </c>
       <c r="C92">
-        <v>0.005851209911202027</v>
+        <v>-6.706708198578326E-05</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="2">
-        <v>45278</v>
+        <v>45287</v>
       </c>
       <c r="B93">
-        <v>-0.007929016424391144</v>
+        <v>-0.001438072982203997</v>
       </c>
       <c r="C93">
-        <v>0.006812752982019665</v>
+        <v>0.004950087244351531</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="2">
-        <v>45275</v>
+        <v>45286</v>
       </c>
       <c r="B94">
-        <v>0.001522359657469163</v>
+        <v>-0.005940594059405946</v>
       </c>
       <c r="C94">
-        <v>-0.004929609758334452</v>
+        <v>0.005875573433368642</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="2">
-        <v>45274</v>
+        <v>45282</v>
       </c>
       <c r="B95">
-        <v>-0.004180125403762225</v>
+        <v>-0.005070626584570803</v>
       </c>
       <c r="C95">
-        <v>0.01063607924921794</v>
+        <v>0.00431980148583011</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="2">
-        <v>45273</v>
+        <v>45281</v>
       </c>
       <c r="B96">
-        <v>-0.010684983781721</v>
+        <v>-0.008918820531488847</v>
       </c>
       <c r="C96">
-        <v>0.02422410860501722</v>
+        <v>0.01053484602917343</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="2">
-        <v>45272</v>
+        <v>45280</v>
       </c>
       <c r="B97">
-        <v>-0.01716489874638383</v>
+        <v>-0.01010101010101017</v>
       </c>
       <c r="C97">
-        <v>-0.004042043556367947</v>
+        <v>-0.007940781639881433</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" s="2">
-        <v>45271</v>
+        <v>45279</v>
       </c>
       <c r="B98">
-        <v>0.008634222919937207</v>
+        <v>-0.01725417439703159</v>
       </c>
       <c r="C98">
-        <v>-0.001400538184336053</v>
+        <v>0.005851209911202027</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="2">
-        <v>45268</v>
+        <v>45278</v>
       </c>
       <c r="B99">
-        <v>-0.01225680933852136</v>
+        <v>-0.007929016424391144</v>
       </c>
       <c r="C99">
-        <v>0.008602491865725037</v>
+        <v>0.006812752982019665</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="2">
-        <v>45267</v>
+        <v>45275</v>
       </c>
       <c r="B100">
-        <v>-0.02028757140043336</v>
+        <v>0.001522359657469163</v>
       </c>
       <c r="C100">
-        <v>0.003080646060036774</v>
+        <v>-0.004929609758334452</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="2">
-        <v>45266</v>
+        <v>45274</v>
       </c>
       <c r="B101">
-        <v>0.003216726980297402</v>
+        <v>-0.004180125403762225</v>
       </c>
       <c r="C101">
-        <v>-0.01008644397689573</v>
+        <v>0.01063607924921794</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="2">
-        <v>45265</v>
+        <v>45273</v>
       </c>
       <c r="B102">
-        <v>0.007414829659318833</v>
+        <v>-0.010684983781721</v>
       </c>
       <c r="C102">
-        <v>0.0007886248748059099</v>
+        <v>0.02422410860501722</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" s="2">
-        <v>45264</v>
+        <v>45272</v>
       </c>
       <c r="B103">
-        <v>0.006564551422319376</v>
+        <v>-0.01716489874638383</v>
       </c>
       <c r="C103">
-        <v>-0.01014808396368549</v>
+        <v>-0.004042043556367947</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" s="2">
-        <v>45261</v>
+        <v>45271</v>
       </c>
       <c r="B104">
-        <v>-0.0005928853754940677</v>
+        <v>0.008634222919937207</v>
       </c>
       <c r="C104">
-        <v>0.006062938326095058</v>
+        <v>-0.001400538184336053</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="2">
-        <v>45260</v>
+        <v>45268</v>
       </c>
       <c r="B105">
-        <v>0.03915364840814717</v>
+        <v>-0.01225680933852136</v>
       </c>
       <c r="C105">
-        <v>0.00975408601042016</v>
+        <v>0.008602491865725037</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="2">
-        <v>45259</v>
+        <v>45267</v>
       </c>
       <c r="B106">
-        <v>0.008753568030447134</v>
+        <v>-0.02028757140043336</v>
       </c>
       <c r="C106">
-        <v>-0.003453508037111419</v>
+        <v>0.003080646060036774</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" s="2">
-        <v>45258</v>
+        <v>45266</v>
       </c>
       <c r="B107">
-        <v>-0.01660064138841721</v>
+        <v>0.003216726980297402</v>
       </c>
       <c r="C107">
-        <v>0.006802829340483596</v>
+        <v>-0.01008644397689573</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="2">
-        <v>45257</v>
+        <v>45265</v>
       </c>
       <c r="B108">
-        <v>0.007481296758104827</v>
+        <v>0.007414829659318833</v>
       </c>
       <c r="C108">
-        <v>0.001123130107852255</v>
+        <v>0.0007886248748059099</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="2">
-        <v>45254</v>
+        <v>45264</v>
       </c>
       <c r="B109">
-        <v>-0.005331302361005319</v>
+        <v>0.006564551422319376</v>
       </c>
       <c r="C109">
-        <v>-0.008169005182657063</v>
+        <v>-0.01014808396368549</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="2">
-        <v>45253</v>
+        <v>45261</v>
       </c>
       <c r="B110">
-        <v>0.00631699846860645</v>
+        <v>-0.0005928853754940677</v>
       </c>
       <c r="C110">
-        <v>0.004292458444083103</v>
+        <v>0.006062938326095058</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="2">
-        <v>45252</v>
+        <v>45260</v>
       </c>
       <c r="B111">
-        <v>-0.0068480121742438</v>
+        <v>0.03915364840814717</v>
       </c>
       <c r="C111">
-        <v>0.003407453406259142</v>
+        <v>0.00975408601042016</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="2">
-        <v>45251</v>
+        <v>45259</v>
       </c>
       <c r="B112">
-        <v>-0.008427504309519218</v>
+        <v>0.008753568030447134</v>
       </c>
       <c r="C112">
-        <v>-0.003870097942027861</v>
+        <v>-0.003453508037111419</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" s="2">
-        <v>45250</v>
+        <v>45258</v>
       </c>
       <c r="B113">
-        <v>-0.00154529650376678</v>
+        <v>-0.01660064138841721</v>
       </c>
       <c r="C113">
-        <v>0.008259903088068343</v>
+        <v>0.006802829340483596</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="2">
-        <v>45247</v>
+        <v>45257</v>
       </c>
       <c r="B114">
-        <v>0.0007738440704196936</v>
+        <v>0.007481296758104827</v>
       </c>
       <c r="C114">
-        <v>0.003901232982275848</v>
+        <v>0.001123130107852255</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" s="2">
-        <v>45246</v>
+        <v>45254</v>
       </c>
       <c r="B115">
-        <v>0.008699014111734016</v>
+        <v>-0.005331302361005319</v>
       </c>
       <c r="C115">
-        <v>0.01011935651271401</v>
+        <v>-0.008169005182657063</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="2">
-        <v>45244</v>
+        <v>45253</v>
       </c>
       <c r="B116">
-        <v>-0.01686469911843624</v>
+        <v>0.00631699846860645</v>
       </c>
       <c r="C116">
-        <v>0.02452316076294281</v>
+        <v>0.004292458444083103</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" s="2">
-        <v>45243</v>
+        <v>45252</v>
       </c>
       <c r="B117">
-        <v>0.03040935672514622</v>
+        <v>-0.0068480121742438</v>
       </c>
       <c r="C117">
-        <v>-0.002155243874133794</v>
+        <v>0.003407453406259142</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="2">
-        <v>45240</v>
+        <v>45251</v>
       </c>
       <c r="B118">
-        <v>0.01002648505486192</v>
+        <v>-0.008427504309519218</v>
       </c>
       <c r="C118">
-        <v>0.01364568278829026</v>
+        <v>-0.003870097942027861</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="2">
-        <v>45239</v>
+        <v>45250</v>
       </c>
       <c r="B119">
-        <v>-0.02210151713804087</v>
+        <v>-0.00154529650376678</v>
       </c>
       <c r="C119">
-        <v>-0.0007304847227936895</v>
+        <v>0.008259903088068343</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="2">
-        <v>45238</v>
+        <v>45247</v>
       </c>
       <c r="B120">
-        <v>0.0009576709442635778</v>
+        <v>0.0007738440704196936</v>
       </c>
       <c r="C120">
-        <v>-0.001416976892376853</v>
+        <v>0.003901232982275848</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="2">
-        <v>45237</v>
+        <v>45246</v>
       </c>
       <c r="B121">
-        <v>-0.02659778032912363</v>
+        <v>0.008699014111734016</v>
       </c>
       <c r="C121">
-        <v>0.006591440411184424</v>
+        <v>0.01011935651271401</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="2">
-        <v>45236</v>
+        <v>45244</v>
       </c>
       <c r="B122">
-        <v>-0.003341851779044558</v>
+        <v>-0.01686469911843624</v>
       </c>
       <c r="C122">
-        <v>0.002767433987813206</v>
+        <v>0.02452316076294281</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="2">
-        <v>45233</v>
+        <v>45243</v>
       </c>
       <c r="B123">
-        <v>-0.01400394477317557</v>
+        <v>0.03040935672514622</v>
       </c>
       <c r="C123">
-        <v>0.02700494554683486</v>
+        <v>-0.002155243874133794</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="2">
-        <v>45231</v>
+        <v>45240</v>
       </c>
       <c r="B124">
-        <v>0.005601120224044909</v>
+        <v>0.01002648505486192</v>
       </c>
       <c r="C124">
-        <v>0.0168723043201584</v>
+        <v>0.01364568278829026</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="2">
-        <v>45230</v>
+        <v>45239</v>
       </c>
       <c r="B125">
-        <v>0.002387109608116056</v>
+        <v>-0.02210151713804087</v>
       </c>
       <c r="C125">
-        <v>0.005438453062240001</v>
+        <v>-0.0007304847227936895</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="2">
-        <v>45229</v>
+        <v>45238</v>
       </c>
       <c r="B126">
-        <v>0.001587616590593255</v>
+        <v>0.0009576709442635778</v>
       </c>
       <c r="C126">
-        <v>-0.006787230474576522</v>
+        <v>-0.001416976892376853</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" s="2">
-        <v>45226</v>
+        <v>45237</v>
       </c>
       <c r="B127">
-        <v>0.005151575193184099</v>
+        <v>-0.02659778032912363</v>
       </c>
       <c r="C127">
-        <v>-0.01285971928173768</v>
+        <v>0.006591440411184424</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" s="2">
-        <v>45225</v>
+        <v>45236</v>
       </c>
       <c r="B128">
-        <v>0.01517839542676924</v>
+        <v>-0.003341851779044558</v>
       </c>
       <c r="C128">
-        <v>0.0172560489231588</v>
+        <v>0.002767433987813206</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" s="2">
-        <v>45224</v>
+        <v>45233</v>
       </c>
       <c r="B129">
-        <v>-0.002135922330097073</v>
+        <v>-0.01400394477317557</v>
       </c>
       <c r="C129">
-        <v>-0.008192542325205276</v>
+        <v>0.02700494554683486</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" s="2">
-        <v>45223</v>
+        <v>45231</v>
       </c>
       <c r="B130">
-        <v>-0.001556723097878909</v>
+        <v>0.005601120224044909</v>
       </c>
       <c r="C130">
-        <v>0.008662499445848404</v>
+        <v>0.0168723043201584</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" s="2">
-        <v>45222</v>
+        <v>45230</v>
       </c>
       <c r="B131">
-        <v>0.03586045605145194</v>
+        <v>0.002387109608116056</v>
       </c>
       <c r="C131">
-        <v>-0.00326985108921396</v>
+        <v>0.005438453062240001</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="2">
-        <v>45219</v>
+        <v>45229</v>
       </c>
       <c r="B132">
-        <v>0.009219190968955848</v>
+        <v>0.001587616590593255</v>
       </c>
       <c r="C132">
-        <v>-0.007447107119048502</v>
+        <v>-0.006787230474576522</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" s="2">
-        <v>45218</v>
+        <v>45226</v>
       </c>
       <c r="B133">
-        <v>0.01976137211036555</v>
+        <v>0.005151575193184099</v>
       </c>
       <c r="C133">
-        <v>-0.0004909696650885476</v>
+        <v>-0.01285971928173768</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" s="2">
-        <v>45217</v>
+        <v>45225</v>
       </c>
       <c r="B134">
-        <v>0.001645338208409397</v>
+        <v>0.01517839542676924</v>
       </c>
       <c r="C134">
-        <v>-0.01594367946992448</v>
+        <v>0.0172560489231588</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" s="2">
-        <v>45216</v>
+        <v>45224</v>
       </c>
       <c r="B135">
-        <v>0.02482204781894515</v>
+        <v>-0.002135922330097073</v>
       </c>
       <c r="C135">
-        <v>-0.005371822815658955</v>
+        <v>-0.008192542325205276</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" s="2">
-        <v>45215</v>
+        <v>45223</v>
       </c>
       <c r="B136">
-        <v>-0.001602849510240367</v>
+        <v>-0.001556723097878909</v>
       </c>
       <c r="C136">
-        <v>0.006738428045683031</v>
+        <v>0.008662499445848404</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="2">
-        <v>45212</v>
+        <v>45222</v>
       </c>
       <c r="B137">
-        <v>0.02069211559043871</v>
+        <v>0.03586045605145194</v>
       </c>
       <c r="C137">
-        <v>-0.01108064006287857</v>
+        <v>-0.00326985108921396</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" s="2">
-        <v>45210</v>
+        <v>45219</v>
       </c>
       <c r="B138">
-        <v>-0.03268088081090526</v>
+        <v>0.009219190968955848</v>
       </c>
       <c r="C138">
-        <v>0.002689807002064448</v>
+        <v>-0.007447107119048502</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" s="2">
-        <v>45209</v>
+        <v>45218</v>
       </c>
       <c r="B139">
-        <v>-0.003432700993676652</v>
+        <v>0.01976137211036555</v>
       </c>
       <c r="C139">
-        <v>0.01372920212581197</v>
+        <v>-0.0004909696650885476</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="2">
-        <v>45208</v>
+        <v>45217</v>
       </c>
       <c r="B140">
-        <v>0.00435097897026826</v>
+        <v>0.001645338208409397</v>
       </c>
       <c r="C140">
-        <v>0.008636244197249621</v>
+        <v>-0.01594367946992448</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="2">
-        <v>45205</v>
+        <v>45216</v>
       </c>
       <c r="B141">
-        <v>-0.008844765342960303</v>
+        <v>0.02482204781894515</v>
       </c>
       <c r="C141">
-        <v>0.007821051516542443</v>
+        <v>-0.005371822815658955</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="2">
-        <v>45204</v>
+        <v>45215</v>
       </c>
       <c r="B142">
-        <v>-0.01675468949189574</v>
+        <v>-0.001602849510240367</v>
       </c>
       <c r="C142">
-        <v>-0.002843134665997726</v>
+        <v>0.006738428045683031</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="2">
-        <v>45203</v>
+        <v>45212</v>
       </c>
       <c r="B143">
-        <v>-0.004630487127245786</v>
+        <v>0.02069211559043871</v>
       </c>
       <c r="C143">
-        <v>0.001657570601045766</v>
+        <v>-0.01108064006287857</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="2">
-        <v>45202</v>
+        <v>45210</v>
       </c>
       <c r="B144">
-        <v>0.005024190547078478</v>
+        <v>-0.03268088081090526</v>
       </c>
       <c r="C144">
-        <v>-0.01423642194738262</v>
+        <v>0.002689807002064448</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="2">
-        <v>45201</v>
+        <v>45209</v>
       </c>
       <c r="B145">
-        <v>-0.01907054249213114</v>
+        <v>-0.003432700993676652</v>
       </c>
       <c r="C145">
-        <v>-0.01293698794663922</v>
+        <v>0.01372920212581197</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="2">
-        <v>45198</v>
+        <v>45208</v>
       </c>
       <c r="B146">
-        <v>0.001132502831257209</v>
+        <v>0.00435097897026826</v>
       </c>
       <c r="C146">
-        <v>0.007206366487803706</v>
+        <v>0.008636244197249621</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="2">
-        <v>45197</v>
+        <v>45205</v>
       </c>
       <c r="B147">
-        <v>-0.008295625942684737</v>
+        <v>-0.008844765342960303</v>
       </c>
       <c r="C147">
-        <v>0.01228056364638275</v>
+        <v>0.007821051516542443</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="2">
-        <v>45196</v>
+        <v>45204</v>
       </c>
       <c r="B148">
-        <v>0.004372623574144363</v>
+        <v>-0.01675468949189574</v>
       </c>
       <c r="C148">
-        <v>0.00117345196290497</v>
+        <v>-0.002843134665997726</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="2">
-        <v>45195</v>
+        <v>45203</v>
       </c>
       <c r="B149">
-        <v>0.005300018928638961</v>
+        <v>-0.004630487127245786</v>
       </c>
       <c r="C149">
-        <v>-0.01494069441449208</v>
+        <v>0.001657570601045766</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="2">
-        <v>45194</v>
+        <v>45202</v>
       </c>
       <c r="B150">
-        <v>0.015627942007155</v>
+        <v>0.005024190547078478</v>
       </c>
       <c r="C150">
-        <v>-0.0007240817522778942</v>
+        <v>-0.01423642194738262</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" s="2">
-        <v>45191</v>
+        <v>45201</v>
       </c>
       <c r="B151">
-        <v>0.003151649981461002</v>
+        <v>-0.01907054249213114</v>
       </c>
       <c r="C151">
-        <v>-0.001170950105471635</v>
+        <v>-0.01293698794663922</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" s="2">
-        <v>45190</v>
+        <v>45198</v>
       </c>
       <c r="B152">
-        <v>0.0114581408242469</v>
+        <v>0.001132502831257209</v>
       </c>
       <c r="C152">
-        <v>-0.02148363452546442</v>
+        <v>0.007206366487803706</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" s="2">
-        <v>45189</v>
+        <v>45197</v>
       </c>
       <c r="B153">
-        <v>-0.02009866617942613</v>
+        <v>-0.008295625942684737</v>
       </c>
       <c r="C153">
-        <v>0.007204317499108992</v>
+        <v>0.01228056364638275</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" s="2">
-        <v>45188</v>
+        <v>45196</v>
       </c>
       <c r="B154">
-        <v>-0.0384113369382808</v>
+        <v>0.004372623574144363</v>
       </c>
       <c r="C154">
-        <v>-0.003736642770188037</v>
+        <v>0.00117345196290497</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" s="2">
-        <v>45187</v>
+        <v>45195</v>
       </c>
       <c r="B155">
-        <v>-0.0137676943959667</v>
+        <v>0.005300018928638961</v>
       </c>
       <c r="C155">
-        <v>-0.003957628117684742</v>
+        <v>-0.01494069441449208</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" s="2">
-        <v>45184</v>
+        <v>45194</v>
       </c>
       <c r="B156">
-        <v>0.009241053873377814</v>
+        <v>0.015627942007155</v>
       </c>
       <c r="C156">
-        <v>-0.0053102385419459</v>
+        <v>-0.0007240817522778942</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" s="2">
-        <v>45183</v>
+        <v>45191</v>
       </c>
       <c r="B157">
-        <v>-0.02474186635495801</v>
+        <v>0.003151649981461002</v>
       </c>
       <c r="C157">
-        <v>0.01028973734091521</v>
+        <v>-0.001170950105471635</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" s="2">
-        <v>45182</v>
+        <v>45190</v>
       </c>
       <c r="B158">
-        <v>-0.0191769876148622</v>
+        <v>0.0114581408242469</v>
       </c>
       <c r="C158">
-        <v>0.00176319001763181</v>
+        <v>-0.02148363452546442</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" s="2">
-        <v>45181</v>
+        <v>45189</v>
       </c>
       <c r="B159">
-        <v>0.0004073319755599769</v>
+        <v>-0.02009866617942613</v>
       </c>
       <c r="C159">
-        <v>0.009282787060564734</v>
+        <v>0.007204317499108992</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" s="2">
-        <v>45180</v>
+        <v>45188</v>
       </c>
       <c r="B160">
-        <v>-0.006107491856677472</v>
+        <v>-0.0384113369382808</v>
       </c>
       <c r="C160">
-        <v>0.01361511711602326</v>
+        <v>-0.003736642770188037</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" s="2">
-        <v>45177</v>
+        <v>45187</v>
       </c>
       <c r="B161">
-        <v>-0.02693877551020407</v>
+        <v>-0.0137676943959667</v>
       </c>
       <c r="C161">
-        <v>-0.005793852653360299</v>
+        <v>-0.003957628117684742</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" s="2">
-        <v>45175</v>
+        <v>45184</v>
       </c>
       <c r="B162">
-        <v>0.02181208053691264</v>
+        <v>0.009241053873377814</v>
       </c>
       <c r="C162">
-        <v>-0.0114718190418559</v>
+        <v>-0.0053102385419459</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" s="2">
-        <v>45174</v>
+        <v>45183</v>
       </c>
       <c r="B163">
-        <v>0.01621510673234816</v>
+        <v>-0.02474186635495801</v>
       </c>
       <c r="C163">
-        <v>-0.003786817460115333</v>
+        <v>0.01028973734091521</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" s="2">
-        <v>45173</v>
+        <v>45182</v>
       </c>
       <c r="B164">
-        <v>0.005857402544940493</v>
+        <v>-0.0191769876148622</v>
       </c>
       <c r="C164">
-        <v>-0.0009839430670184335</v>
+        <v>0.00176319001763181</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" s="2">
-        <v>45170</v>
+        <v>45181</v>
       </c>
       <c r="B165">
-        <v>-0.02385141739980445</v>
+        <v>0.0004073319755599769</v>
       </c>
       <c r="C165">
-        <v>0.01858443780131669</v>
+        <v>0.009282787060564734</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" s="2">
-        <v>45169</v>
+        <v>45180</v>
       </c>
       <c r="B166">
-        <v>-0.0186260765071099</v>
+        <v>-0.006107491856677472</v>
       </c>
       <c r="C166">
-        <v>-0.01525503041647169</v>
+        <v>0.01361511711602326</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="2">
-        <v>45168</v>
+        <v>45177</v>
       </c>
       <c r="B167">
-        <v>0.01367346938775515</v>
+        <v>-0.02693877551020407</v>
       </c>
       <c r="C167">
-        <v>-0.007339279078409477</v>
+        <v>-0.005793852653360299</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="2">
-        <v>45167</v>
+        <v>45175</v>
       </c>
       <c r="B168">
-        <v>0.006241191866317664</v>
+        <v>0.02181208053691264</v>
       </c>
       <c r="C168">
-        <v>0.01095448297060297</v>
+        <v>-0.0114718190418559</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" s="2">
-        <v>45166</v>
+        <v>45174</v>
       </c>
       <c r="B169">
-        <v>-0.0166066426570628</v>
+        <v>0.01621510673234816</v>
       </c>
       <c r="C169">
-        <v>0.01108454120876745</v>
+        <v>-0.003786817460115333</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="2">
-        <v>45163</v>
+        <v>45173</v>
       </c>
       <c r="B170">
-        <v>-0.007934893184130209</v>
+        <v>0.005857402544940493</v>
       </c>
       <c r="C170">
-        <v>-0.01016013535453664</v>
+        <v>-0.0009839430670184335</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="2">
-        <v>45162</v>
+        <v>45170</v>
       </c>
       <c r="B171">
-        <v>-0.01107465135356844</v>
+        <v>-0.02385141739980445</v>
       </c>
       <c r="C171">
-        <v>-0.009387565073856186</v>
+        <v>0.01858443780131669</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" s="2">
-        <v>45161</v>
+        <v>45169</v>
       </c>
       <c r="B172">
-        <v>0.002695976773123165</v>
+        <v>-0.0186260765071099</v>
       </c>
       <c r="C172">
-        <v>0.01703743241847167</v>
+        <v>-0.01525503041647169</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" s="2">
-        <v>45160</v>
+        <v>45168</v>
       </c>
       <c r="B173">
-        <v>0.007445708376421889</v>
+        <v>0.01367346938775515</v>
       </c>
       <c r="C173">
-        <v>0.0150923279937778</v>
+        <v>-0.007339279078409477</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" s="2">
-        <v>45159</v>
+        <v>45167</v>
       </c>
       <c r="B174">
-        <v>0.004516526380619945</v>
+        <v>0.006241191866317664</v>
       </c>
       <c r="C174">
-        <v>-0.008491538788136133</v>
+        <v>0.01095448297060297</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" s="2">
-        <v>45156</v>
+        <v>45166</v>
       </c>
       <c r="B175">
-        <v>0.01205804210096062</v>
+        <v>-0.0166066426570628</v>
       </c>
       <c r="C175">
-        <v>0.00371362474126391</v>
+        <v>0.01108454120876745</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" s="2">
-        <v>45155</v>
+        <v>45163</v>
       </c>
       <c r="B176">
-        <v>-0.005452342487883732</v>
+        <v>-0.007934893184130209</v>
       </c>
       <c r="C176">
-        <v>-0.005277181811890075</v>
+        <v>-0.01016013535453664</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" s="2">
-        <v>45154</v>
+        <v>45162</v>
       </c>
       <c r="B177">
-        <v>-0.009746192893400951</v>
+        <v>-0.01107465135356844</v>
       </c>
       <c r="C177">
-        <v>-0.00498403215948906</v>
+        <v>-0.009387565073856186</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" s="2">
-        <v>45153</v>
+        <v>45161</v>
       </c>
       <c r="B178">
-        <v>0.002460529013737833</v>
+        <v>0.002695976773123165</v>
       </c>
       <c r="C178">
-        <v>-0.005470422052906376</v>
+        <v>0.01703743241847167</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" s="2">
-        <v>45152</v>
+        <v>45160</v>
       </c>
       <c r="B179">
-        <v>0.01759050930660666</v>
+        <v>0.007445708376421889</v>
       </c>
       <c r="C179">
-        <v>-0.01062973785626564</v>
+        <v>0.0150923279937778</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" s="2">
-        <v>45149</v>
+        <v>45159</v>
       </c>
       <c r="B180">
-        <v>-0.01467336683417075</v>
+        <v>0.004516526380619945</v>
       </c>
       <c r="C180">
-        <v>-0.002408111533586776</v>
+        <v>-0.008491538788136133</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" s="2">
-        <v>45148</v>
+        <v>45156</v>
       </c>
       <c r="B181">
-        <v>-0.01631986944104458</v>
+        <v>0.01205804210096062</v>
       </c>
       <c r="C181">
-        <v>-0.0004982729353343318</v>
+        <v>0.00371362474126391</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" s="2">
-        <v>45147</v>
+        <v>45155</v>
       </c>
       <c r="B182">
-        <v>-0.001036914143508816</v>
+        <v>-0.005452342487883732</v>
       </c>
       <c r="C182">
-        <v>-0.005718364262322639</v>
+        <v>-0.005277181811890075</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" s="2">
-        <v>45146</v>
+        <v>45154</v>
       </c>
       <c r="B183">
-        <v>0.009134315964293149</v>
+        <v>-0.009746192893400951</v>
       </c>
       <c r="C183">
-        <v>-0.002429217624392743</v>
+        <v>-0.00498403215948906</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" s="2">
-        <v>45145</v>
+        <v>45153</v>
       </c>
       <c r="B184">
-        <v>0.01542892408969343</v>
+        <v>0.002460529013737833</v>
       </c>
       <c r="C184">
-        <v>-0.001071058004485037</v>
+        <v>-0.005470422052906376</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" s="2">
-        <v>45142</v>
+        <v>45152</v>
       </c>
       <c r="B185">
-        <v>-0.004862236628849326</v>
+        <v>0.01759050930660666</v>
       </c>
       <c r="C185">
-        <v>-0.00893967790622463</v>
+        <v>-0.01062973785626564</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" s="2">
-        <v>45141</v>
+        <v>45149</v>
       </c>
       <c r="B186">
-        <v>-0.0126221498371335</v>
+        <v>-0.01467336683417075</v>
       </c>
       <c r="C186">
-        <v>-0.002258830538064971</v>
+        <v>-0.002408111533586776</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" s="2">
-        <v>45140</v>
+        <v>45148</v>
       </c>
       <c r="B187">
-        <v>-0.03525773195876292</v>
+        <v>-0.01631986944104458</v>
       </c>
       <c r="C187">
-        <v>-0.003208300343098491</v>
+        <v>-0.0004982729353343318</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" s="2">
-        <v>45139</v>
+        <v>45147</v>
       </c>
       <c r="B188">
-        <v>0.0102586022654414</v>
+        <v>-0.001036914143508816</v>
       </c>
       <c r="C188">
-        <v>-0.005699384138490915</v>
+        <v>-0.005718364262322639</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" s="2">
-        <v>45138</v>
+        <v>45146</v>
       </c>
       <c r="B189">
-        <v>-0.006346519991538013</v>
+        <v>0.009134315964293149</v>
       </c>
       <c r="C189">
-        <v>0.01461056520255943</v>
+        <v>-0.002429217624392743</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" s="2">
-        <v>45135</v>
+        <v>45145</v>
       </c>
       <c r="B190">
-        <v>-0.0178837555886735</v>
+        <v>0.01542892408969343</v>
       </c>
       <c r="C190">
-        <v>0.001641803483623638</v>
+        <v>-0.001071058004485037</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" s="2">
-        <v>45134</v>
+        <v>45142</v>
       </c>
       <c r="B191">
-        <v>-0.0002167786689790674</v>
+        <v>-0.004862236628849326</v>
       </c>
       <c r="C191">
-        <v>-0.0209693211488251</v>
+        <v>-0.00893967790622463</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" s="2">
-        <v>45133</v>
+        <v>45141</v>
       </c>
       <c r="B192">
-        <v>-0.01539462272333048</v>
+        <v>-0.0126221498371335</v>
       </c>
       <c r="C192">
-        <v>0.004524293488951558</v>
+        <v>-0.002258830538064971</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="2">
-        <v>45132</v>
+        <v>45140</v>
       </c>
       <c r="B193">
-        <v>-0.02686632900242236</v>
+        <v>-0.03525773195876292</v>
       </c>
       <c r="C193">
-        <v>0.005488618944800683</v>
+        <v>-0.003208300343098491</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="2">
-        <v>45131</v>
+        <v>45139</v>
       </c>
       <c r="B194">
-        <v>-0.004525910839556335</v>
+        <v>0.0102586022654414</v>
       </c>
       <c r="C194">
-        <v>0.009358077476563142</v>
+        <v>-0.005699384138490915</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" s="2">
-        <v>45128</v>
+        <v>45138</v>
       </c>
       <c r="B195">
-        <v>-0.02136849283928177</v>
+        <v>-0.006346519991538013</v>
       </c>
       <c r="C195">
-        <v>0.01807203407772495</v>
+        <v>0.01461056520255943</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" s="2">
-        <v>45127</v>
+        <v>45135</v>
       </c>
       <c r="B196">
-        <v>-0.009291521486643362</v>
+        <v>-0.0178837555886735</v>
       </c>
       <c r="C196">
-        <v>0.004517149857084624</v>
+        <v>0.001641803483623638</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" s="2">
-        <v>45126</v>
+        <v>45134</v>
       </c>
       <c r="B197">
-        <v>-0.004220398593200447</v>
+        <v>-0.0002167786689790674</v>
       </c>
       <c r="C197">
-        <v>-0.002452457124430429</v>
+        <v>-0.0209693211488251</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" s="2">
-        <v>45125</v>
+        <v>45133</v>
       </c>
       <c r="B198">
-        <v>0.02542971509300673</v>
+        <v>-0.01539462272333048</v>
       </c>
       <c r="C198">
-        <v>-0.003197455569747709</v>
+        <v>0.004524293488951558</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" s="2">
-        <v>45124</v>
+        <v>45132</v>
       </c>
       <c r="B199">
-        <v>-0.00390355912743956</v>
+        <v>-0.02686632900242236</v>
       </c>
       <c r="C199">
-        <v>0.004315654441810812</v>
+        <v>0.005488618944800683</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" s="2">
-        <v>45121</v>
+        <v>45131</v>
       </c>
       <c r="B200">
-        <v>0.003457814661134151</v>
+        <v>-0.004525910839556335</v>
       </c>
       <c r="C200">
-        <v>-0.01302153206332168</v>
+        <v>0.009358077476563142</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" s="2">
-        <v>45120</v>
+        <v>45128</v>
       </c>
       <c r="B201">
-        <v>-0.004135079255685681</v>
+        <v>-0.02136849283928177</v>
       </c>
       <c r="C201">
-        <v>0.01358081348902829</v>
+        <v>0.01807203407772495</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" s="2">
-        <v>45119</v>
+        <v>45127</v>
       </c>
       <c r="B202">
-        <v>-0.004152249134948049</v>
+        <v>-0.009291521486643362</v>
       </c>
       <c r="C202">
-        <v>0.003804811465620173</v>
+        <v>0.004517149857084624</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" s="2">
-        <v>45118</v>
+        <v>45126</v>
       </c>
       <c r="B203">
-        <v>-0.003011350474866892</v>
+        <v>-0.004220398593200447</v>
       </c>
       <c r="C203">
-        <v>-0.006121653015889184</v>
+        <v>-0.002452457124430429</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" s="2">
-        <v>45117</v>
+        <v>45125</v>
       </c>
       <c r="B204">
-        <v>-0.0004646840148697651</v>
+        <v>0.02542971509300673</v>
       </c>
       <c r="C204">
-        <v>-0.008040505307069901</v>
+        <v>-0.003197455569747709</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" s="2">
-        <v>45114</v>
+        <v>45124</v>
       </c>
       <c r="B205">
-        <v>0.01092515109251502</v>
+        <v>-0.00390355912743956</v>
       </c>
       <c r="C205">
-        <v>0.01253555430654196</v>
+        <v>0.004315654441810812</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" s="2">
-        <v>45113</v>
+        <v>45121</v>
       </c>
       <c r="B206">
-        <v>-0.008967578753736549</v>
+        <v>0.003457814661134151</v>
       </c>
       <c r="C206">
-        <v>-0.01775840868597811</v>
+        <v>-0.01302153206332168</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" s="2">
-        <v>45112</v>
+        <v>45120</v>
       </c>
       <c r="B207">
-        <v>0.007656612529002293</v>
+        <v>-0.004135079255685681</v>
       </c>
       <c r="C207">
-        <v>0.003972253014881355</v>
+        <v>0.01358081348902829</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" s="2">
-        <v>45111</v>
+        <v>45119</v>
       </c>
       <c r="B208">
-        <v>0.006447156343541316</v>
+        <v>-0.004152249134948049</v>
       </c>
       <c r="C208">
-        <v>-0.004988593918427764</v>
+        <v>0.003804811465620173</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" s="2">
-        <v>45110</v>
+        <v>45118</v>
       </c>
       <c r="B209">
-        <v>-0.01143902997025847</v>
+        <v>-0.003011350474866892</v>
       </c>
       <c r="C209">
-        <v>0.01343077561458927</v>
+        <v>-0.006121653015889184</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" s="2">
-        <v>45107</v>
+        <v>45117</v>
       </c>
       <c r="B210">
-        <v>0</v>
+        <v>-0.0004646840148697651</v>
       </c>
       <c r="C210">
-        <v>-0.002500359004248942</v>
+        <v>-0.008040505307069901</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" s="2">
-        <v>45106</v>
+        <v>45114</v>
       </c>
       <c r="B211">
-        <v>-0.003934274473501587</v>
+        <v>0.01092515109251502</v>
       </c>
       <c r="C211">
-        <v>0.01458677933853836</v>
+        <v>0.01253555430654196</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" s="2">
-        <v>45105</v>
+        <v>45113</v>
       </c>
       <c r="B212">
-        <v>0.002788104089219257</v>
+        <v>-0.008967578753736549</v>
       </c>
       <c r="C212">
-        <v>-0.007164555023272068</v>
+        <v>-0.01775840868597811</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" s="2">
-        <v>45104</v>
+        <v>45112</v>
       </c>
       <c r="B213">
-        <v>0.01506024096385561</v>
+        <v>0.007656612529002293</v>
       </c>
       <c r="C213">
-        <v>-0.006089155383405376</v>
+        <v>0.003972253014881355</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" s="2">
-        <v>45103</v>
+        <v>45111</v>
       </c>
       <c r="B214">
-        <v>0.01711937913718331</v>
+        <v>0.006447156343541316</v>
       </c>
       <c r="C214">
-        <v>-0.006169259604797528</v>
+        <v>-0.004988593918427764</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" s="2">
-        <v>45100</v>
+        <v>45110</v>
       </c>
       <c r="B215">
-        <v>0.007405745062836644</v>
+        <v>-0.01143902997025847</v>
       </c>
       <c r="C215">
-        <v>0.0003615450586038627</v>
+        <v>0.01343077561458927</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" s="2">
-        <v>45099</v>
+        <v>45107</v>
       </c>
       <c r="B216">
-        <v>-0.00178213410559136</v>
+        <v>0</v>
       </c>
       <c r="C216">
-        <v>-0.01234014283341633</v>
+        <v>-0.002500359004248942</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" s="2">
-        <v>45098</v>
+        <v>45106</v>
       </c>
       <c r="B217">
-        <v>0.01338986833296119</v>
+        <v>-0.003934274473501587</v>
       </c>
       <c r="C217">
-        <v>0.006671013693133387</v>
+        <v>0.01458677933853836</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" s="2">
-        <v>45097</v>
+        <v>45105</v>
       </c>
       <c r="B218">
-        <v>0.02070028628055498</v>
+        <v>0.002788104089219257</v>
       </c>
       <c r="C218">
-        <v>-0.001968996646031118</v>
+        <v>-0.007164555023272068</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" s="2">
-        <v>45096</v>
+        <v>45104</v>
       </c>
       <c r="B219">
-        <v>0.005609492988133624</v>
+        <v>0.01506024096385561</v>
       </c>
       <c r="C219">
-        <v>0.009262533892453462</v>
+        <v>-0.006089155383405376</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" s="2">
-        <v>45093</v>
+        <v>45103</v>
       </c>
       <c r="B220">
-        <v>0.01244368161338771</v>
+        <v>0.01711937913718331</v>
       </c>
       <c r="C220">
-        <v>-0.003883544006508921</v>
+        <v>-0.006169259604797528</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" s="2">
-        <v>45092</v>
+        <v>45100</v>
       </c>
       <c r="B221">
-        <v>0.0008476372112735664</v>
+        <v>0.007405745062836644</v>
       </c>
       <c r="C221">
-        <v>0.001276570727897219</v>
+        <v>0.0003615450586038627</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" s="2">
-        <v>45091</v>
+        <v>45099</v>
       </c>
       <c r="B222">
-        <v>-0.03493542240101633</v>
+        <v>-0.00178213410559136</v>
       </c>
       <c r="C222">
-        <v>0.01992410679869461</v>
+        <v>-0.01234014283341633</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" s="2">
-        <v>45090</v>
+        <v>45098</v>
       </c>
       <c r="B223">
-        <v>0.008556384379113657</v>
+        <v>0.01338986833296119</v>
       </c>
       <c r="C223">
-        <v>-0.005053862412217947</v>
+        <v>0.006671013693133387</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" s="2">
-        <v>45089</v>
+        <v>45097</v>
       </c>
       <c r="B224">
-        <v>-0.007396127909506167</v>
+        <v>0.02070028628055498</v>
       </c>
       <c r="C224">
-        <v>0.00270896179252933</v>
+        <v>-0.001968996646031118</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" s="2">
-        <v>45086</v>
+        <v>45096</v>
       </c>
       <c r="B225">
-        <v>-0.03133903133903138</v>
+        <v>0.005609492988133624</v>
       </c>
       <c r="C225">
-        <v>0.01325678858409529</v>
+        <v>0.009262533892453462</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" s="2">
-        <v>45084</v>
+        <v>45093</v>
       </c>
       <c r="B226">
-        <v>0.01312217194570131</v>
+        <v>0.01244368161338771</v>
       </c>
       <c r="C226">
-        <v>0.007660762586161773</v>
+        <v>-0.003883544006508921</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" s="2">
-        <v>45083</v>
+        <v>45092</v>
       </c>
       <c r="B227">
-        <v>0.02411790978115236</v>
+        <v>0.0008476372112735664</v>
       </c>
       <c r="C227">
-        <v>0.0169837438773337</v>
+        <v>0.001276570727897219</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" s="2">
-        <v>45082</v>
+        <v>45091</v>
       </c>
       <c r="B228">
-        <v>-0.002616659398168242</v>
+        <v>-0.03493542240101633</v>
       </c>
       <c r="C228">
-        <v>0.001226034577728852</v>
+        <v>0.01992410679869461</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" s="2">
-        <v>45079</v>
+        <v>45090</v>
       </c>
       <c r="B229">
-        <v>-0.008307826847398392</v>
+        <v>0.008556384379113657</v>
       </c>
       <c r="C229">
-        <v>0.01802559580337348</v>
+        <v>-0.005053862412217947</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" s="2">
-        <v>45078</v>
+        <v>45089</v>
       </c>
       <c r="B230">
-        <v>-0.03064373897707229</v>
+        <v>-0.007396127909506167</v>
       </c>
       <c r="C230">
-        <v>0.02058429870309686</v>
+        <v>0.00270896179252933</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" s="2">
-        <v>45077</v>
+        <v>45086</v>
       </c>
       <c r="B231">
-        <v>-0.005003411416875103</v>
+        <v>-0.03133903133903138</v>
       </c>
       <c r="C231">
-        <v>-0.005799921077023318</v>
+        <v>0.01325678858409529</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" s="2">
-        <v>45076</v>
+        <v>45084</v>
       </c>
       <c r="B232">
-        <v>0.00777142857142854</v>
+        <v>0.01312217194570131</v>
       </c>
       <c r="C232">
-        <v>-0.01238070205650166</v>
+        <v>0.007660762586161773</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" s="2">
-        <v>45075</v>
+        <v>45083</v>
       </c>
       <c r="B233">
-        <v>0.005670220004536208</v>
+        <v>0.02411790978115236</v>
       </c>
       <c r="C233">
-        <v>-0.005166537428092255</v>
+        <v>0.0169837438773337</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" s="2">
-        <v>45072</v>
+        <v>45082</v>
       </c>
       <c r="B234">
-        <v>-0.0006765899864682456</v>
+        <v>-0.002616659398168242</v>
       </c>
       <c r="C234">
-        <v>0.007741654097079609</v>
+        <v>0.001226034577728852</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" s="2">
-        <v>45071</v>
+        <v>45079</v>
       </c>
       <c r="B235">
-        <v>-0.02708192281652</v>
+        <v>-0.008307826847398392</v>
       </c>
       <c r="C235">
-        <v>0.0115257352941176</v>
+        <v>0.01802559580337348</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" s="2">
-        <v>45070</v>
+        <v>45078</v>
       </c>
       <c r="B236">
-        <v>0.01067037810252836</v>
+        <v>-0.03064373897707229</v>
       </c>
       <c r="C236">
-        <v>-0.0102702653530915</v>
+        <v>0.02058429870309686</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" s="2">
-        <v>45069</v>
+        <v>45077</v>
       </c>
       <c r="B237">
-        <v>0.02845994950654118</v>
+        <v>-0.005003411416875103</v>
       </c>
       <c r="C237">
-        <v>-0.00257682850480434</v>
+        <v>-0.005799921077023318</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" s="2">
-        <v>45068</v>
+        <v>45076</v>
       </c>
       <c r="B238">
-        <v>-0.01495201963847359</v>
+        <v>0.00777142857142854</v>
       </c>
       <c r="C238">
-        <v>-0.004803828615287387</v>
+        <v>-0.01238070205650166</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" s="2">
-        <v>45065</v>
+        <v>45075</v>
       </c>
       <c r="B239">
-        <v>0.005437245129134682</v>
+        <v>0.005670220004536208</v>
       </c>
       <c r="C239">
-        <v>0.005785229047843954</v>
+        <v>-0.005166537428092255</v>
       </c>
     </row>
     <row r="240" spans="1:3">
       <c r="A240" s="2">
-        <v>45064</v>
+        <v>45072</v>
       </c>
       <c r="B240">
-        <v>-0.001577287066246047</v>
+        <v>-0.0006765899864682456</v>
       </c>
       <c r="C240">
-        <v>0.005919970765576377</v>
+        <v>0.007741654097079609</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" s="2">
-        <v>45063</v>
+        <v>45071</v>
       </c>
       <c r="B241">
-        <v>-0.03565786504175139</v>
+        <v>-0.02708192281652</v>
       </c>
       <c r="C241">
-        <v>0.01170120339390346</v>
+        <v>0.0115257352941176</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" s="2">
+        <v>45070</v>
+      </c>
+      <c r="B242">
+        <v>0.01067037810252836</v>
+      </c>
+      <c r="C242">
+        <v>-0.0102702653530915</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3">
+      <c r="A243" s="2">
+        <v>45069</v>
+      </c>
+      <c r="B243">
+        <v>0.02845994950654118</v>
+      </c>
+      <c r="C243">
+        <v>-0.00257682850480434</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3">
+      <c r="A244" s="2">
+        <v>45068</v>
+      </c>
+      <c r="B244">
+        <v>-0.01495201963847359</v>
+      </c>
+      <c r="C244">
+        <v>-0.004803828615287387</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3">
+      <c r="A245" s="2">
+        <v>45065</v>
+      </c>
+      <c r="B245">
+        <v>0.005437245129134682</v>
+      </c>
+      <c r="C245">
+        <v>0.005785229047843954</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3">
+      <c r="A246" s="2">
+        <v>45064</v>
+      </c>
+      <c r="B246">
+        <v>-0.001577287066246047</v>
+      </c>
+      <c r="C246">
+        <v>0.005919970765576377</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3">
+      <c r="A247" s="2">
+        <v>45063</v>
+      </c>
+      <c r="B247">
+        <v>-0.03565786504175139</v>
+      </c>
+      <c r="C247">
+        <v>0.01170120339390346</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3">
+      <c r="A248" s="2">
         <v>45062</v>
       </c>
-      <c r="B242">
+      <c r="B248">
         <v>-0.0004680552305170727</v>
       </c>
-      <c r="C242">
+      <c r="C248">
         <v>-0.007658512872721901</v>
       </c>
     </row>
@@ -3081,7 +3147,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-0.2957109638466428</v>
+        <v>-0.3182495238079706</v>
       </c>
     </row>
   </sheetData>

</xml_diff>